<commit_message>
trying to improve cupy performance
</commit_message>
<xml_diff>
--- a/benchmarks_tests/performance.xlsx
+++ b/benchmarks_tests/performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/CP_IV/Exercise4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manas\Documents\crysx_nn\benchmarks_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E397D98-16BC-304B-8CA2-1FB475E7700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386AC629-2DB8-4FBC-90A7-DB6264D5F06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="880" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{F8ACF7B6-A719-5A49-89C3-B4340F0ED991}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="5" xr2:uid="{F8ACF7B6-A719-5A49-89C3-B4340F0ED991}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
   <si>
     <t>Model</t>
   </si>
@@ -162,6 +163,9 @@
   <si>
     <t>500,500,500,500,500,500,500,1</t>
   </si>
+  <si>
+    <t>MNIST Kaggle</t>
+  </si>
 </sst>
 </file>
 
@@ -249,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -296,9 +300,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -325,6 +326,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,7 +352,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1314,7 +1321,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2300,7 +2307,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5051,13 +5058,13 @@
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -5073,9 +5080,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+    <row r="2" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="2">
         <v>-6</v>
       </c>
@@ -5089,7 +5096,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -5117,7 +5124,7 @@
         <v>0.74933687002652527</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -5145,7 +5152,7 @@
         <v>0.81582952815829535</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -5173,7 +5180,7 @@
         <v>1.218707015130674</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -5201,7 +5208,7 @@
         <v>2.3654822335025383</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -5229,7 +5236,7 @@
         <v>3.408450704225352</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="36.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
@@ -5275,19 +5282,19 @@
       <selection activeCell="A3" sqref="A3:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="2" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65"/>
+    <row r="3" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -5303,9 +5310,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+    <row r="4" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="2">
         <v>6</v>
       </c>
@@ -5315,7 +5322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -5343,7 +5350,7 @@
         <v>0.57610619469026547</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -5371,7 +5378,7 @@
         <v>0.81743227326266199</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -5399,7 +5406,7 @@
         <v>1.1304347826086958</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5427,7 +5434,7 @@
         <v>1.9189189189189189</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
@@ -5455,7 +5462,7 @@
         <v>2.9223300970873787</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="36.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
@@ -5500,23 +5507,23 @@
       <selection activeCell="A5" sqref="A5:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -5532,9 +5539,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+    <row r="4" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="2">
         <v>6.5</v>
       </c>
@@ -5544,7 +5551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -5572,7 +5579,7 @@
         <v>0.58921568627450982</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -5600,7 +5607,7 @@
         <v>0.70272727272727276</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -5628,7 +5635,7 @@
         <v>0.78028747433264878</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5656,7 +5663,7 @@
         <v>0.86473429951690817</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
@@ -5684,7 +5691,7 @@
         <v>1.4787234042553192</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="36.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
@@ -5730,23 +5737,23 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -5762,9 +5769,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+    <row r="4" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="2">
         <v>6</v>
       </c>
@@ -5778,7 +5785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -5806,7 +5813,7 @@
         <v>0.70844686648501365</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -5834,7 +5841,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -5862,7 +5869,7 @@
         <v>1.330357142857143</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -5890,7 +5897,7 @@
         <v>1.2417218543046358</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="54.9" x14ac:dyDescent="0.6">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
@@ -5918,7 +5925,7 @@
         <v>0.94612068965517238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="55.2" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -5946,23 +5953,23 @@
         <v>0.85666666666666669</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:8" ht="73.2" x14ac:dyDescent="0.6">
+      <c r="A11" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="25">
         <v>1505001</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="18">
         <v>76</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>71</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="18">
         <v>60</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="18">
         <v>64</v>
       </c>
       <c r="G11">
@@ -5988,13 +5995,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55B451C-30A0-2146-8D94-EFD11E3F197D}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -6002,7 +6009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -6016,7 +6023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -6030,21 +6037,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:8" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -6060,9 +6067,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
+    <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="2">
         <v>7</v>
       </c>
@@ -6076,11 +6083,11 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A8" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>8070</v>
       </c>
       <c r="C8" s="4">
@@ -6104,8 +6111,8 @@
         <v>1.0535714285714284</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A9" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="6">
@@ -6132,8 +6139,8 @@
         <v>1.3383838383838382</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="40" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A10" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="8">
@@ -6160,8 +6167,8 @@
         <v>1.407258064516129</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A11" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="6">
@@ -6188,36 +6195,36 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>1047210</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="24">
         <v>148</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <v>431</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="24">
         <v>218</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="24">
         <v>103</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
         <v>1.472972972972973</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="21">
         <f t="shared" si="1"/>
         <v>2.116504854368932</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="41" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:8" ht="36.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A13" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="10">
@@ -6244,8 +6251,8 @@
         <v>2.6645569620253164</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
+    <row r="14" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A14" s="18"/>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -6259,4 +6266,273 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FA1CC5-7431-4E08-8B84-CED1C73BE227}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A6" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="2">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="20">
+        <v>8070</v>
+      </c>
+      <c r="C8" s="4">
+        <v>41</v>
+      </c>
+      <c r="D8" s="4">
+        <v>14.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>17.7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>16.8</v>
+      </c>
+      <c r="G8">
+        <f>E8/C8</f>
+        <v>0.43170731707317073</v>
+      </c>
+      <c r="H8">
+        <f>E8/F8</f>
+        <v>1.0535714285714284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6">
+        <v>42310</v>
+      </c>
+      <c r="C9" s="5">
+        <v>53.1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>26.7</v>
+      </c>
+      <c r="E9" s="5">
+        <v>26.5</v>
+      </c>
+      <c r="F9" s="5">
+        <v>19.8</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G12" si="0">E9/C9</f>
+        <v>0.49905838041431261</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H12" si="1">E9/F9</f>
+        <v>1.3383838383838382</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="8">
+        <v>89610</v>
+      </c>
+      <c r="C10" s="7">
+        <v>60</v>
+      </c>
+      <c r="D10" s="7">
+        <v>54.2</v>
+      </c>
+      <c r="E10" s="7">
+        <v>34.9</v>
+      </c>
+      <c r="F10" s="7">
+        <v>24.8</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.58166666666666667</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1.407258064516129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="6">
+        <v>648010</v>
+      </c>
+      <c r="C11" s="5">
+        <v>107</v>
+      </c>
+      <c r="D11" s="5">
+        <v>379</v>
+      </c>
+      <c r="E11" s="5">
+        <v>138</v>
+      </c>
+      <c r="F11" s="5">
+        <v>75</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1.2897196261682242</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="23">
+        <v>1047210</v>
+      </c>
+      <c r="C12" s="24">
+        <v>148</v>
+      </c>
+      <c r="D12" s="24">
+        <v>431</v>
+      </c>
+      <c r="E12" s="24">
+        <v>218</v>
+      </c>
+      <c r="F12" s="24">
+        <v>103</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1.472972972972973</v>
+      </c>
+      <c r="H12" s="21">
+        <f t="shared" si="1"/>
+        <v>2.116504854368932</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="36.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A13" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="10">
+        <v>1796010</v>
+      </c>
+      <c r="C13" s="9">
+        <v>171</v>
+      </c>
+      <c r="D13" s="9">
+        <v>758</v>
+      </c>
+      <c r="E13" s="9">
+        <v>421</v>
+      </c>
+      <c r="F13" s="9">
+        <v>158</v>
+      </c>
+      <c r="G13">
+        <f>E13/C13</f>
+        <v>2.4619883040935671</v>
+      </c>
+      <c r="H13">
+        <f>E13/F13</f>
+        <v>2.6645569620253164</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
the gpu benchmark of pytorch was not set to use cuda before. now it is fixed
</commit_message>
<xml_diff>
--- a/benchmarks_tests/performance.xlsx
+++ b/benchmarks_tests/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manas\Documents\crysx_nn\benchmarks_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386AC629-2DB8-4FBC-90A7-DB6264D5F06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0098A7DD-A96A-44AE-A678-C67CA83B472C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="5" xr2:uid="{F8ACF7B6-A719-5A49-89C3-B4340F0ED991}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="3" xr2:uid="{F8ACF7B6-A719-5A49-89C3-B4340F0ED991}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1071,7 +1071,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1106,7 +1106,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1044362976"/>
@@ -1183,7 +1183,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1218,7 +1218,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1043972896"/>
@@ -1259,7 +1259,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1307,7 +1307,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1426,7 +1426,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2057,7 +2057,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2092,7 +2092,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1556245167"/>
@@ -2169,7 +2169,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2204,7 +2204,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1556138383"/>
@@ -2245,7 +2245,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2293,7 +2293,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2319,6 +2319,41 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Wall time (s) vs no. of paramaters</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2332,11 +2367,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -2344,7 +2378,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2369,27 +2403,41 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2474,27 +2522,41 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2579,27 +2641,41 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2684,27 +2760,41 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2796,9 +2886,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2806,6 +2897,64 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" b="1" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>No. of parameters</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2814,9 +2963,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2830,9 +2978,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2840,7 +2987,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1556696991"/>
@@ -2858,9 +3005,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2868,6 +3016,64 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" b="1" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Wall time (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2876,9 +3082,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2892,9 +3097,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2902,7 +3106,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1556158431"/>
@@ -2918,7 +3122,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2934,9 +3138,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -2944,7 +3147,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2961,11 +3164,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -2981,7 +3187,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4117,56 +4323,46 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -4174,16 +4370,15 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4193,23 +4388,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -4217,63 +4407,123 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:effectRef idx="0">
       <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -4297,21 +4547,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4321,20 +4568,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4346,14 +4592,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4365,14 +4610,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4384,14 +4628,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -4403,9 +4641,10 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4422,9 +4661,10 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4436,14 +4676,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4455,14 +4694,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4474,27 +4712,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -4502,9 +4739,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4514,14 +4750,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4533,12 +4768,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4547,14 +4781,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4563,9 +4798,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4575,17 +4809,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4597,37 +4832,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -5054,7 +5282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD795A89-CE30-594C-A97F-8F0109C7BED8}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
@@ -5733,8 +5961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC3E7F9-E984-8646-AB0A-67841AF15C8D}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -6272,7 +6500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FA1CC5-7431-4E08-8B84-CED1C73BE227}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>